<commit_message>
Refs #19042 : Use correct xlsx files for rating factors and super group specs.
</commit_message>
<xml_diff>
--- a/spec/test_data/plan_data/super_groups/Fallon 2017 Super Groups_Connector.xlsx
+++ b/spec/test_data/plan_data/super_groups/Fallon 2017 Super Groups_Connector.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11017"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vsonnathi/Projects/ma/enroll/spec/test_data/plan_data/super_groups/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vsonnathi/Projects/ma/enroll/lib/xls_templates/super_groups/2017/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="108">
   <si>
     <t>Plan Year</t>
   </si>
@@ -74,17 +74,290 @@
     <t>Standard</t>
   </si>
   <si>
+    <t>88806MA0040003-01</t>
+  </si>
+  <si>
+    <t>Business Express - 4 Tier</t>
+  </si>
+  <si>
+    <t>88806MA0030003-01</t>
+  </si>
+  <si>
+    <t>88806MA0040005-01</t>
+  </si>
+  <si>
+    <t>88806MA0030004-01</t>
+  </si>
+  <si>
+    <t>88806MA0040006-01</t>
+  </si>
+  <si>
+    <t>88806MA0030006-01</t>
+  </si>
+  <si>
+    <t>88806MA0040008-01</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>88806MA0030100-01</t>
+  </si>
+  <si>
+    <t>88806MA0040051-01</t>
+  </si>
+  <si>
+    <t>88806MA0010001-01</t>
+  </si>
+  <si>
+    <t>Direct Care HMO</t>
+  </si>
+  <si>
+    <t>Narrow</t>
+  </si>
+  <si>
+    <t>88806MA0020003-01</t>
+  </si>
+  <si>
+    <t>88806MA0010003-01</t>
+  </si>
+  <si>
+    <t>88806MA0020005-01</t>
+  </si>
+  <si>
+    <t>88806MA0010004-01</t>
+  </si>
+  <si>
+    <t>88806MA0020006-01</t>
+  </si>
+  <si>
+    <t>88806MA0010006-01</t>
+  </si>
+  <si>
+    <t>88806MA0020008-01</t>
+  </si>
+  <si>
+    <t>88806MA0010010-01</t>
+  </si>
+  <si>
+    <t>88806MA0010096-01</t>
+  </si>
+  <si>
+    <t>individual, Non-Group</t>
+  </si>
+  <si>
+    <t>88806MA0020045-01</t>
+  </si>
+  <si>
+    <t>88806MA0010100-01</t>
+  </si>
+  <si>
+    <t>88806MA0020051-01</t>
+  </si>
+  <si>
+    <t>Community Care HMO</t>
+  </si>
+  <si>
+    <t>Community Care Wrap Type III</t>
+  </si>
+  <si>
+    <t>Community Care Wrap Type II</t>
+  </si>
+  <si>
+    <t>Community Care Wrap Type I</t>
+  </si>
+  <si>
+    <t>88806MA0040053-01</t>
+  </si>
+  <si>
     <t xml:space="preserve">Standard Platinum: Select Care Platinum Connector </t>
   </si>
   <si>
+    <t xml:space="preserve">Standard Platinum: Direct Care Platinum Connector </t>
+  </si>
+  <si>
+    <t>Non-Standard: Select Care Gold Connector A</t>
+  </si>
+  <si>
+    <t>Non-Standard: Direct Care Gold Connector A</t>
+  </si>
+  <si>
+    <t>Standard Gold: Select Care Fallon Gold Connector B</t>
+  </si>
+  <si>
+    <t>Standard Gold: Direct Care Gold Connector B</t>
+  </si>
+  <si>
+    <t>Non-Standard: Direct Care Deductible 2000 Hybrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard Silver: Select Care Silver Connector </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard Silver: Direct Care Silver Connector </t>
+  </si>
+  <si>
+    <t>Non-Standard: Select Care Silver Coinsurance 35%</t>
+  </si>
+  <si>
+    <t>88806MA0030102-01</t>
+  </si>
+  <si>
+    <t>Non-Standard: Select Care Bronze Deductible 3000</t>
+  </si>
+  <si>
+    <t>Non-Standard: Direct Care Bronze Deductible 3000</t>
+  </si>
+  <si>
+    <t>Standard: Direct Care Catastrophic Plan</t>
+  </si>
+  <si>
+    <t>88806MA0090002-01</t>
+  </si>
+  <si>
+    <t>88806MA0100002-01</t>
+  </si>
+  <si>
+    <t>Non-Standard: Community Care Silver Coinsurance 35%</t>
+  </si>
+  <si>
+    <t>Frozen</t>
+  </si>
+  <si>
+    <t>88806MA0030101-01</t>
+  </si>
+  <si>
+    <t>88806MA0040052-01</t>
+  </si>
+  <si>
+    <t>Standard Bronze: Select Care Bronze Connector</t>
+  </si>
+  <si>
+    <t>88806MA0010101-01</t>
+  </si>
+  <si>
+    <t>88806MA0020052-01</t>
+  </si>
+  <si>
+    <t>Standard Bronze: Direct Care Bronze Connector</t>
+  </si>
+  <si>
+    <t>88806MA0090002-04</t>
+  </si>
+  <si>
+    <t>88806MA0090002-05</t>
+  </si>
+  <si>
+    <t>88806MA0090002-06</t>
+  </si>
+  <si>
     <t>X226</t>
+  </si>
+  <si>
+    <t>X227</t>
+  </si>
+  <si>
+    <t>XH249</t>
+  </si>
+  <si>
+    <t>XH250</t>
+  </si>
+  <si>
+    <t>XH253</t>
+  </si>
+  <si>
+    <t>XH254</t>
+  </si>
+  <si>
+    <t>XH257</t>
+  </si>
+  <si>
+    <t>XH258</t>
+  </si>
+  <si>
+    <t>XH245</t>
+  </si>
+  <si>
+    <t>XH246</t>
+  </si>
+  <si>
+    <t>XH261</t>
+  </si>
+  <si>
+    <t>XH262</t>
+  </si>
+  <si>
+    <t>XH265</t>
+  </si>
+  <si>
+    <t>XH266</t>
+  </si>
+  <si>
+    <t>X228</t>
+  </si>
+  <si>
+    <t>X229</t>
+  </si>
+  <si>
+    <t>XH251</t>
+  </si>
+  <si>
+    <t>XH252</t>
+  </si>
+  <si>
+    <t>XH255</t>
+  </si>
+  <si>
+    <t>XH256</t>
+  </si>
+  <si>
+    <t>XH259</t>
+  </si>
+  <si>
+    <t>XH260</t>
+  </si>
+  <si>
+    <t>XH269</t>
+  </si>
+  <si>
+    <t>XH243</t>
+  </si>
+  <si>
+    <t>XH244</t>
+  </si>
+  <si>
+    <t>XH247</t>
+  </si>
+  <si>
+    <t>XH248</t>
+  </si>
+  <si>
+    <t>XH267</t>
+  </si>
+  <si>
+    <t>XH268</t>
+  </si>
+  <si>
+    <t>C109</t>
+  </si>
+  <si>
+    <t>C110</t>
+  </si>
+  <si>
+    <t>C113</t>
+  </si>
+  <si>
+    <t>C112</t>
+  </si>
+  <si>
+    <t>C111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,7 +399,19 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -182,10 +467,10 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -210,6 +495,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,8 +526,8 @@
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 14" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 10" xfId="3"/>
+    <cellStyle name="Normal 14" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -520,14 +828,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD35"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -536,11 +844,11 @@
     <col min="2" max="2" width="21.5" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="56.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.6640625" style="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" style="24" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
@@ -584,13 +892,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>12</v>
@@ -600,6 +908,929 @@
       </c>
       <c r="I2" s="11" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A33" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A34" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A35" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>